<commit_message>
v0.2.2 - Added Online/Presential
</commit_message>
<xml_diff>
--- a/Inputs/University.xlsx
+++ b/Inputs/University.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hbonn\Desktop\ESILV\A4\PI2\GitHub_PI2\Inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02EC4600-AC54-43E5-A189-AFD86A0D8EF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C76B88BC-8088-4B89-A83C-9BFEBDAFC0B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{B72B09E8-A954-412D-973D-4D6537A5C659}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{B72B09E8-A954-412D-973D-4D6537A5C659}"/>
   </bookViews>
   <sheets>
     <sheet name="University" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="112">
   <si>
     <t>Name</t>
   </si>
@@ -124,265 +124,259 @@
     <t>L102</t>
   </si>
   <si>
+    <t>default</t>
+  </si>
+  <si>
+    <t>Setting</t>
+  </si>
+  <si>
+    <t>Value</t>
+  </si>
+  <si>
+    <t>Start day</t>
+  </si>
+  <si>
+    <t>Start month</t>
+  </si>
+  <si>
+    <t>Start year</t>
+  </si>
+  <si>
+    <t>Days</t>
+  </si>
+  <si>
+    <t>StartH</t>
+  </si>
+  <si>
+    <t>StartMin</t>
+  </si>
+  <si>
+    <t>EndH</t>
+  </si>
+  <si>
+    <t>EndMin</t>
+  </si>
+  <si>
+    <t>Subjects (séparés d'un '-')</t>
+  </si>
+  <si>
+    <t>Henri</t>
+  </si>
+  <si>
+    <t>Barbeau</t>
+  </si>
+  <si>
+    <t>Timothé</t>
+  </si>
+  <si>
+    <t>Solé</t>
+  </si>
+  <si>
+    <t>Renaud</t>
+  </si>
+  <si>
+    <t>Cerfbeer</t>
+  </si>
+  <si>
+    <t>Christiane</t>
+  </si>
+  <si>
+    <t>Brunelle</t>
+  </si>
+  <si>
+    <t>Constantin</t>
+  </si>
+  <si>
+    <t>Poussin</t>
+  </si>
+  <si>
+    <t>Maurice</t>
+  </si>
+  <si>
+    <t>Vannier</t>
+  </si>
+  <si>
+    <t>Napoléon</t>
+  </si>
+  <si>
+    <t>Matthieu</t>
+  </si>
+  <si>
+    <t>Josette</t>
+  </si>
+  <si>
+    <t>Paquin</t>
+  </si>
+  <si>
+    <t>Achille</t>
+  </si>
+  <si>
+    <t>Cochet</t>
+  </si>
+  <si>
+    <t>Henry</t>
+  </si>
+  <si>
+    <t>D'Aboville</t>
+  </si>
+  <si>
+    <t>A3</t>
+  </si>
+  <si>
+    <t>UNI014</t>
+  </si>
+  <si>
+    <t>Basic Chemistry</t>
+  </si>
+  <si>
+    <t>UNI015</t>
+  </si>
+  <si>
+    <t>Basic Biology</t>
+  </si>
+  <si>
+    <t>UNI016</t>
+  </si>
+  <si>
+    <t>Basic Engineering</t>
+  </si>
+  <si>
+    <t>UNI024</t>
+  </si>
+  <si>
+    <t>Advanced Chemistry</t>
+  </si>
+  <si>
+    <t>UNI025</t>
+  </si>
+  <si>
+    <t>Advanced Biology</t>
+  </si>
+  <si>
+    <t>UNI026</t>
+  </si>
+  <si>
+    <t>Advanced Engineering</t>
+  </si>
+  <si>
+    <t>UNI031</t>
+  </si>
+  <si>
+    <t>Applied Mathematics</t>
+  </si>
+  <si>
+    <t>UNI032</t>
+  </si>
+  <si>
+    <t>Quantum Mechanics</t>
+  </si>
+  <si>
+    <t>UNI033</t>
+  </si>
+  <si>
+    <t>Artificial Intelligence</t>
+  </si>
+  <si>
+    <t>UNI034</t>
+  </si>
+  <si>
+    <t>Organic Chemistry</t>
+  </si>
+  <si>
+    <t>UNI035</t>
+  </si>
+  <si>
+    <t>Genetics</t>
+  </si>
+  <si>
+    <t>UNI036</t>
+  </si>
+  <si>
+    <t>Mechanical Systems</t>
+  </si>
+  <si>
+    <t>FF33A8</t>
+  </si>
+  <si>
+    <t>33FF57</t>
+  </si>
+  <si>
+    <t>33A8FF</t>
+  </si>
+  <si>
+    <t>FFD700</t>
+  </si>
+  <si>
+    <t>FF8C00</t>
+  </si>
+  <si>
+    <t>DC143C</t>
+  </si>
+  <si>
+    <t>8A2BE2</t>
+  </si>
+  <si>
+    <t>00FA9A</t>
+  </si>
+  <si>
+    <t>1E90FF</t>
+  </si>
+  <si>
+    <t>FF4500</t>
+  </si>
+  <si>
+    <t>FF5733</t>
+  </si>
+  <si>
+    <t>UNI011-UNI021-UNI031-UNI041-UNI051</t>
+  </si>
+  <si>
+    <t>UNI012-UNI022-UNI032-UNI042-UNI052</t>
+  </si>
+  <si>
+    <t>UNI013-UNI023-UNI033-UNI043-UNI053</t>
+  </si>
+  <si>
+    <t>UNI014-UNI024-UNI034-UNI044-UNI054</t>
+  </si>
+  <si>
+    <t>UNI015-UNI025-UNI035-UNI045-UNI055</t>
+  </si>
+  <si>
+    <t>UNI016-UNI026-UNI036-UNI046-UNI056</t>
+  </si>
+  <si>
+    <t>John</t>
+  </si>
+  <si>
+    <t>Doe</t>
+  </si>
+  <si>
+    <t>David</t>
+  </si>
+  <si>
+    <t>Brown</t>
+  </si>
+  <si>
+    <t>FF1493</t>
+  </si>
+  <si>
+    <t>9932CC</t>
+  </si>
+  <si>
+    <t>00CED1</t>
+  </si>
+  <si>
+    <t>4682B4</t>
+  </si>
+  <si>
+    <t>FFA500</t>
+  </si>
+  <si>
+    <t>Online</t>
+  </si>
+  <si>
     <t>L103</t>
-  </si>
-  <si>
-    <t>L104</t>
-  </si>
-  <si>
-    <t>L105</t>
-  </si>
-  <si>
-    <t>default</t>
-  </si>
-  <si>
-    <t>Setting</t>
-  </si>
-  <si>
-    <t>Value</t>
-  </si>
-  <si>
-    <t>Start day</t>
-  </si>
-  <si>
-    <t>Start month</t>
-  </si>
-  <si>
-    <t>Start year</t>
-  </si>
-  <si>
-    <t>Days</t>
-  </si>
-  <si>
-    <t>StartH</t>
-  </si>
-  <si>
-    <t>StartMin</t>
-  </si>
-  <si>
-    <t>EndH</t>
-  </si>
-  <si>
-    <t>EndMin</t>
-  </si>
-  <si>
-    <t>Subjects (séparés d'un '-')</t>
-  </si>
-  <si>
-    <t>Henri</t>
-  </si>
-  <si>
-    <t>Barbeau</t>
-  </si>
-  <si>
-    <t>Timothé</t>
-  </si>
-  <si>
-    <t>Solé</t>
-  </si>
-  <si>
-    <t>Renaud</t>
-  </si>
-  <si>
-    <t>Cerfbeer</t>
-  </si>
-  <si>
-    <t>Christiane</t>
-  </si>
-  <si>
-    <t>Brunelle</t>
-  </si>
-  <si>
-    <t>Constantin</t>
-  </si>
-  <si>
-    <t>Poussin</t>
-  </si>
-  <si>
-    <t>Maurice</t>
-  </si>
-  <si>
-    <t>Vannier</t>
-  </si>
-  <si>
-    <t>Napoléon</t>
-  </si>
-  <si>
-    <t>Matthieu</t>
-  </si>
-  <si>
-    <t>Josette</t>
-  </si>
-  <si>
-    <t>Paquin</t>
-  </si>
-  <si>
-    <t>Achille</t>
-  </si>
-  <si>
-    <t>Cochet</t>
-  </si>
-  <si>
-    <t>Henry</t>
-  </si>
-  <si>
-    <t>D'Aboville</t>
-  </si>
-  <si>
-    <t>A3</t>
-  </si>
-  <si>
-    <t>UNI014</t>
-  </si>
-  <si>
-    <t>Basic Chemistry</t>
-  </si>
-  <si>
-    <t>UNI015</t>
-  </si>
-  <si>
-    <t>Basic Biology</t>
-  </si>
-  <si>
-    <t>UNI016</t>
-  </si>
-  <si>
-    <t>Basic Engineering</t>
-  </si>
-  <si>
-    <t>UNI024</t>
-  </si>
-  <si>
-    <t>Advanced Chemistry</t>
-  </si>
-  <si>
-    <t>UNI025</t>
-  </si>
-  <si>
-    <t>Advanced Biology</t>
-  </si>
-  <si>
-    <t>UNI026</t>
-  </si>
-  <si>
-    <t>Advanced Engineering</t>
-  </si>
-  <si>
-    <t>UNI031</t>
-  </si>
-  <si>
-    <t>Applied Mathematics</t>
-  </si>
-  <si>
-    <t>UNI032</t>
-  </si>
-  <si>
-    <t>Quantum Mechanics</t>
-  </si>
-  <si>
-    <t>UNI033</t>
-  </si>
-  <si>
-    <t>Artificial Intelligence</t>
-  </si>
-  <si>
-    <t>UNI034</t>
-  </si>
-  <si>
-    <t>Organic Chemistry</t>
-  </si>
-  <si>
-    <t>UNI035</t>
-  </si>
-  <si>
-    <t>Genetics</t>
-  </si>
-  <si>
-    <t>UNI036</t>
-  </si>
-  <si>
-    <t>Mechanical Systems</t>
-  </si>
-  <si>
-    <t>FF33A8</t>
-  </si>
-  <si>
-    <t>33FF57</t>
-  </si>
-  <si>
-    <t>33A8FF</t>
-  </si>
-  <si>
-    <t>FFD700</t>
-  </si>
-  <si>
-    <t>FF8C00</t>
-  </si>
-  <si>
-    <t>DC143C</t>
-  </si>
-  <si>
-    <t>8A2BE2</t>
-  </si>
-  <si>
-    <t>00FA9A</t>
-  </si>
-  <si>
-    <t>1E90FF</t>
-  </si>
-  <si>
-    <t>FF4500</t>
-  </si>
-  <si>
-    <t>FF5733</t>
-  </si>
-  <si>
-    <t>UNI011-UNI021-UNI031-UNI041-UNI051</t>
-  </si>
-  <si>
-    <t>UNI012-UNI022-UNI032-UNI042-UNI052</t>
-  </si>
-  <si>
-    <t>UNI013-UNI023-UNI033-UNI043-UNI053</t>
-  </si>
-  <si>
-    <t>UNI014-UNI024-UNI034-UNI044-UNI054</t>
-  </si>
-  <si>
-    <t>UNI015-UNI025-UNI035-UNI045-UNI055</t>
-  </si>
-  <si>
-    <t>UNI016-UNI026-UNI036-UNI046-UNI056</t>
-  </si>
-  <si>
-    <t>John</t>
-  </si>
-  <si>
-    <t>Doe</t>
-  </si>
-  <si>
-    <t>David</t>
-  </si>
-  <si>
-    <t>Brown</t>
-  </si>
-  <si>
-    <t>L106</t>
-  </si>
-  <si>
-    <t>FF1493</t>
-  </si>
-  <si>
-    <t>9932CC</t>
-  </si>
-  <si>
-    <t>00CED1</t>
-  </si>
-  <si>
-    <t>4682B4</t>
-  </si>
-  <si>
-    <t>FFA500</t>
   </si>
 </sst>
 </file>
@@ -763,7 +757,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42AB5D4C-C765-4C0B-97C4-EF4AAF1E2B40}">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
@@ -771,10 +765,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -787,7 +781,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B3">
         <v>6</v>
@@ -795,7 +789,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -803,7 +797,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B5">
         <v>2025</v>
@@ -811,10 +805,10 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B6">
-        <v>60</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -834,16 +828,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D1" t="s">
         <v>37</v>
-      </c>
-      <c r="B1" t="s">
-        <v>38</v>
-      </c>
-      <c r="C1" t="s">
-        <v>39</v>
-      </c>
-      <c r="D1" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
@@ -951,27 +945,33 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49E3E0C2-CBFD-441F-AB28-E61B30CAF7BA}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>3</v>
       </c>
       <c r="B1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>4</v>
       </c>
       <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
         <v>4</v>
       </c>
     </row>
@@ -985,7 +985,7 @@
   <dimension ref="A1:E31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1025,7 +1025,7 @@
         <v>12</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
@@ -1042,7 +1042,7 @@
         <v>15</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
@@ -1059,15 +1059,15 @@
         <v>12</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>3</v>
@@ -1076,15 +1076,15 @@
         <v>15</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>3</v>
@@ -1093,15 +1093,15 @@
         <v>9</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>3</v>
@@ -1110,7 +1110,7 @@
         <v>15</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
@@ -1127,7 +1127,7 @@
         <v>12</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
@@ -1144,7 +1144,7 @@
         <v>15</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
@@ -1161,15 +1161,15 @@
         <v>12</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>2</v>
@@ -1178,15 +1178,15 @@
         <v>12</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>2</v>
@@ -1195,15 +1195,15 @@
         <v>12</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>2</v>
@@ -1212,109 +1212,109 @@
         <v>15</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="D14" s="1">
         <v>24</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="D15" s="1">
         <v>27</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="D16" s="1">
         <v>27</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="D17" s="1">
         <v>30</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="D18" s="1">
         <v>21</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="D19" s="1">
         <v>30</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
@@ -1382,7 +1382,7 @@
         <v>22</v>
       </c>
       <c r="D1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
@@ -1390,13 +1390,13 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D2" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
@@ -1404,13 +1404,13 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C3" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D3" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
@@ -1418,13 +1418,13 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C4" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
@@ -1432,13 +1432,13 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C5" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -1446,13 +1446,13 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C6" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
@@ -1460,13 +1460,13 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C7" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
@@ -1474,13 +1474,13 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C8" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="D8" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
@@ -1488,13 +1488,13 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C9" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="D9" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
@@ -1502,13 +1502,13 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C10" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="D10" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
@@ -1516,13 +1516,13 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C11" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="D11" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
@@ -1530,13 +1530,13 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="C12" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="D12" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
@@ -1544,13 +1544,13 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="C13" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="D13" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
@@ -1563,10 +1563,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E13FFBB7-0715-45C0-A6D5-76680980035E}">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1584,7 +1584,7 @@
         <v>25</v>
       </c>
       <c r="B2" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -1592,39 +1592,23 @@
         <v>26</v>
       </c>
       <c r="B3" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
+        <v>111</v>
+      </c>
+      <c r="B4" t="s">
         <v>27</v>
-      </c>
-      <c r="B4" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>28</v>
+        <v>110</v>
       </c>
       <c r="B5" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>29</v>
-      </c>
-      <c r="B6" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>108</v>
-      </c>
-      <c r="B7" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
v0.2.4 - Visual timetable
</commit_message>
<xml_diff>
--- a/Inputs/University.xlsx
+++ b/Inputs/University.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hbonn\Desktop\ESILV\A4\PI2\GitHub_PI2\Inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C76B88BC-8088-4B89-A83C-9BFEBDAFC0B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{672D9157-A123-40A2-B44C-B2ED4FE6DF72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{B72B09E8-A954-412D-973D-4D6537A5C659}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{B72B09E8-A954-412D-973D-4D6537A5C659}"/>
   </bookViews>
   <sheets>
     <sheet name="University" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="112">
   <si>
     <t>Name</t>
   </si>
@@ -757,7 +757,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42AB5D4C-C765-4C0B-97C4-EF4AAF1E2B40}">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
@@ -945,33 +945,27 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49E3E0C2-CBFD-441F-AB28-E61B30CAF7BA}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>3</v>
       </c>
       <c r="B1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>

<commit_message>
v0.3.1 - Minimizing gaps
</commit_message>
<xml_diff>
--- a/Inputs/University.xlsx
+++ b/Inputs/University.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hbonn\Desktop\ESILV\A4\PI2\GitHub_PI2\Inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC4A4E9F-C391-40D2-9DBA-B614E0D5F979}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98581DB9-5264-41A8-9B0F-FC17F67FAEAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28890" yWindow="-3720" windowWidth="23010" windowHeight="12210" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-34170" yWindow="-2700" windowWidth="24255" windowHeight="16575" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="University" sheetId="1" r:id="rId1"/>
@@ -379,193 +379,193 @@
     <t>A3</t>
   </si>
   <si>
+    <t>TDB</t>
+  </si>
+  <si>
+    <t>UNI014</t>
+  </si>
+  <si>
+    <t>Basic Chemistry</t>
+  </si>
+  <si>
+    <t>33A8FF</t>
+  </si>
+  <si>
+    <t>UNI015</t>
+  </si>
+  <si>
+    <t>Basic Biology</t>
+  </si>
+  <si>
+    <t>FFD700</t>
+  </si>
+  <si>
+    <t>UNI016</t>
+  </si>
+  <si>
+    <t>Basic Engineering</t>
+  </si>
+  <si>
+    <t>FF8C00</t>
+  </si>
+  <si>
+    <t>UNI024</t>
+  </si>
+  <si>
+    <t>Advanced Chemistry</t>
+  </si>
+  <si>
+    <t>1E90FF</t>
+  </si>
+  <si>
+    <t>UNI025</t>
+  </si>
+  <si>
+    <t>Advanced Biology</t>
+  </si>
+  <si>
+    <t>UNI026</t>
+  </si>
+  <si>
+    <t>Advanced Engineering</t>
+  </si>
+  <si>
+    <t>FF4500</t>
+  </si>
+  <si>
+    <t>UNI031</t>
+  </si>
+  <si>
+    <t>Applied Mathematics</t>
+  </si>
+  <si>
+    <t>FF1493</t>
+  </si>
+  <si>
+    <t>UNI032</t>
+  </si>
+  <si>
+    <t>Quantum Mechanics</t>
+  </si>
+  <si>
+    <t>9932CC</t>
+  </si>
+  <si>
+    <t>UNI033</t>
+  </si>
+  <si>
+    <t>Artificial Intelligence</t>
+  </si>
+  <si>
+    <t>00CED1</t>
+  </si>
+  <si>
+    <t>UNI034</t>
+  </si>
+  <si>
+    <t>Organic Chemistry</t>
+  </si>
+  <si>
+    <t>4682B4</t>
+  </si>
+  <si>
+    <t>UNI035</t>
+  </si>
+  <si>
+    <t>Genetics</t>
+  </si>
+  <si>
+    <t>FFA500</t>
+  </si>
+  <si>
+    <t>UNI036</t>
+  </si>
+  <si>
+    <t>Mechanical Systems</t>
+  </si>
+  <si>
+    <t>UNI011-UNI021-UNI031-UNI041-UNI051</t>
+  </si>
+  <si>
+    <t>UNI012-UNI022-UNI032-UNI042-UNI052</t>
+  </si>
+  <si>
+    <t>Achille</t>
+  </si>
+  <si>
+    <t>Cochet</t>
+  </si>
+  <si>
+    <t>Henry</t>
+  </si>
+  <si>
+    <t>UNI013-UNI023-UNI033-UNI043-UNI053</t>
+  </si>
+  <si>
+    <t>UNI014-UNI024-UNI034-UNI044-UNI054</t>
+  </si>
+  <si>
+    <t>Napoléon</t>
+  </si>
+  <si>
+    <t>Matthieu</t>
+  </si>
+  <si>
+    <t>UNI015-UNI025-UNI035-UNI045-UNI055</t>
+  </si>
+  <si>
+    <t>Josette</t>
+  </si>
+  <si>
+    <t>Paquin</t>
+  </si>
+  <si>
+    <t>John</t>
+  </si>
+  <si>
+    <t>Doe</t>
+  </si>
+  <si>
+    <t>UNI016-UNI026-UNI036-UNI046-UNI056</t>
+  </si>
+  <si>
+    <t>David</t>
+  </si>
+  <si>
+    <t>Brown</t>
+  </si>
+  <si>
+    <t>DAboville</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>9</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>11</t>
+  </si>
+  <si>
+    <t>L104</t>
+  </si>
+  <si>
+    <t>L105</t>
+  </si>
+  <si>
+    <t>L106</t>
+  </si>
+  <si>
     <t>TDC</t>
-  </si>
-  <si>
-    <t>TDB</t>
-  </si>
-  <si>
-    <t>UNI014</t>
-  </si>
-  <si>
-    <t>Basic Chemistry</t>
-  </si>
-  <si>
-    <t>33A8FF</t>
-  </si>
-  <si>
-    <t>UNI015</t>
-  </si>
-  <si>
-    <t>Basic Biology</t>
-  </si>
-  <si>
-    <t>FFD700</t>
-  </si>
-  <si>
-    <t>UNI016</t>
-  </si>
-  <si>
-    <t>Basic Engineering</t>
-  </si>
-  <si>
-    <t>FF8C00</t>
-  </si>
-  <si>
-    <t>UNI024</t>
-  </si>
-  <si>
-    <t>Advanced Chemistry</t>
-  </si>
-  <si>
-    <t>1E90FF</t>
-  </si>
-  <si>
-    <t>UNI025</t>
-  </si>
-  <si>
-    <t>Advanced Biology</t>
-  </si>
-  <si>
-    <t>UNI026</t>
-  </si>
-  <si>
-    <t>Advanced Engineering</t>
-  </si>
-  <si>
-    <t>FF4500</t>
-  </si>
-  <si>
-    <t>UNI031</t>
-  </si>
-  <si>
-    <t>Applied Mathematics</t>
-  </si>
-  <si>
-    <t>FF1493</t>
-  </si>
-  <si>
-    <t>UNI032</t>
-  </si>
-  <si>
-    <t>Quantum Mechanics</t>
-  </si>
-  <si>
-    <t>9932CC</t>
-  </si>
-  <si>
-    <t>UNI033</t>
-  </si>
-  <si>
-    <t>Artificial Intelligence</t>
-  </si>
-  <si>
-    <t>00CED1</t>
-  </si>
-  <si>
-    <t>UNI034</t>
-  </si>
-  <si>
-    <t>Organic Chemistry</t>
-  </si>
-  <si>
-    <t>4682B4</t>
-  </si>
-  <si>
-    <t>UNI035</t>
-  </si>
-  <si>
-    <t>Genetics</t>
-  </si>
-  <si>
-    <t>FFA500</t>
-  </si>
-  <si>
-    <t>UNI036</t>
-  </si>
-  <si>
-    <t>Mechanical Systems</t>
-  </si>
-  <si>
-    <t>UNI011-UNI021-UNI031-UNI041-UNI051</t>
-  </si>
-  <si>
-    <t>UNI012-UNI022-UNI032-UNI042-UNI052</t>
-  </si>
-  <si>
-    <t>Achille</t>
-  </si>
-  <si>
-    <t>Cochet</t>
-  </si>
-  <si>
-    <t>Henry</t>
-  </si>
-  <si>
-    <t>UNI013-UNI023-UNI033-UNI043-UNI053</t>
-  </si>
-  <si>
-    <t>UNI014-UNI024-UNI034-UNI044-UNI054</t>
-  </si>
-  <si>
-    <t>Napoléon</t>
-  </si>
-  <si>
-    <t>Matthieu</t>
-  </si>
-  <si>
-    <t>UNI015-UNI025-UNI035-UNI045-UNI055</t>
-  </si>
-  <si>
-    <t>Josette</t>
-  </si>
-  <si>
-    <t>Paquin</t>
-  </si>
-  <si>
-    <t>John</t>
-  </si>
-  <si>
-    <t>Doe</t>
-  </si>
-  <si>
-    <t>UNI016-UNI026-UNI036-UNI046-UNI056</t>
-  </si>
-  <si>
-    <t>David</t>
-  </si>
-  <si>
-    <t>Brown</t>
-  </si>
-  <si>
-    <t>DAboville</t>
-  </si>
-  <si>
-    <t>6</t>
-  </si>
-  <si>
-    <t>7</t>
-  </si>
-  <si>
-    <t>8</t>
-  </si>
-  <si>
-    <t>9</t>
-  </si>
-  <si>
-    <t>10</t>
-  </si>
-  <si>
-    <t>11</t>
-  </si>
-  <si>
-    <t>L104</t>
-  </si>
-  <si>
-    <t>L105</t>
-  </si>
-  <si>
-    <t>L106</t>
   </si>
 </sst>
 </file>
@@ -927,7 +927,7 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+      <selection activeCell="M17" sqref="M17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -977,7 +977,7 @@
         <v>7</v>
       </c>
       <c r="B6">
-        <v>60</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -1114,7 +1114,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
@@ -1154,7 +1154,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B5" t="s">
         <v>14</v>
@@ -1162,7 +1162,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B6" t="s">
         <v>14</v>
@@ -1170,7 +1170,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B7" t="s">
         <v>14</v>
@@ -1193,8 +1193,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1215,10 +1215,10 @@
         <v>20</v>
       </c>
       <c r="B2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C2" t="s">
-        <v>117</v>
+        <v>179</v>
       </c>
     </row>
   </sheetData>
@@ -1312,10 +1312,10 @@
     </row>
     <row r="5" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>119</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>120</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>18</v>
@@ -1324,15 +1324,15 @@
         <v>15</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>122</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>123</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>18</v>
@@ -1341,15 +1341,15 @@
         <v>9</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>125</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>126</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>18</v>
@@ -1358,7 +1358,7 @@
         <v>15</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -1414,10 +1414,10 @@
     </row>
     <row r="11" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="B11" s="2" t="s">
         <v>128</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>129</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>19</v>
@@ -1426,15 +1426,15 @@
         <v>12</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="B12" s="2" t="s">
         <v>131</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>132</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>19</v>
@@ -1443,15 +1443,15 @@
         <v>12</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="B13" s="2" t="s">
         <v>133</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>134</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>19</v>
@@ -1460,15 +1460,15 @@
         <v>15</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="B14" s="2" t="s">
         <v>136</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>137</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>116</v>
@@ -1477,15 +1477,15 @@
         <v>24</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="B15" s="2" t="s">
         <v>139</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>140</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>116</v>
@@ -1494,15 +1494,15 @@
         <v>27</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="B16" s="2" t="s">
         <v>142</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>143</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>116</v>
@@ -1511,15 +1511,15 @@
         <v>27</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="B17" s="2" t="s">
         <v>145</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>146</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>116</v>
@@ -1528,15 +1528,15 @@
         <v>30</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="B18" s="2" t="s">
         <v>148</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>149</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>116</v>
@@ -1545,15 +1545,15 @@
         <v>21</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="B19" s="2" t="s">
         <v>151</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>152</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>116</v>
@@ -1610,7 +1610,7 @@
         <v>48</v>
       </c>
       <c r="D2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -1624,7 +1624,7 @@
         <v>50</v>
       </c>
       <c r="D3" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -1638,7 +1638,7 @@
         <v>52</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="13.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -1646,13 +1646,13 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
+        <v>154</v>
+      </c>
+      <c r="C5" t="s">
         <v>155</v>
       </c>
-      <c r="C5" t="s">
-        <v>156</v>
-      </c>
       <c r="D5" s="2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -1660,13 +1660,13 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
+        <v>156</v>
+      </c>
+      <c r="C6" t="s">
+        <v>169</v>
+      </c>
+      <c r="D6" s="2" t="s">
         <v>157</v>
-      </c>
-      <c r="C6" t="s">
-        <v>170</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>158</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -1680,7 +1680,7 @@
         <v>54</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
@@ -1694,7 +1694,7 @@
         <v>56</v>
       </c>
       <c r="D8" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
@@ -1708,7 +1708,7 @@
         <v>58</v>
       </c>
       <c r="D9" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
@@ -1716,13 +1716,13 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
+        <v>159</v>
+      </c>
+      <c r="C10" t="s">
         <v>160</v>
       </c>
-      <c r="C10" t="s">
+      <c r="D10" t="s">
         <v>161</v>
-      </c>
-      <c r="D10" t="s">
-        <v>162</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
@@ -1730,13 +1730,13 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
+        <v>162</v>
+      </c>
+      <c r="C11" t="s">
         <v>163</v>
       </c>
-      <c r="C11" t="s">
-        <v>164</v>
-      </c>
       <c r="D11" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
@@ -1744,13 +1744,13 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
+        <v>164</v>
+      </c>
+      <c r="C12" t="s">
         <v>165</v>
       </c>
-      <c r="C12" t="s">
+      <c r="D12" t="s">
         <v>166</v>
-      </c>
-      <c r="D12" t="s">
-        <v>167</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -1758,13 +1758,13 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
+        <v>167</v>
+      </c>
+      <c r="C13" t="s">
         <v>168</v>
       </c>
-      <c r="C13" t="s">
-        <v>169</v>
-      </c>
       <c r="D13" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
   </sheetData>
@@ -2852,7 +2852,7 @@
     </row>
     <row r="8" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B8">
         <v>1</v>
@@ -3004,7 +3004,7 @@
     </row>
     <row r="9" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -3156,7 +3156,7 @@
     </row>
     <row r="10" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B10">
         <v>1</v>
@@ -3308,7 +3308,7 @@
     </row>
     <row r="11" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B11">
         <v>1</v>
@@ -3460,7 +3460,7 @@
     </row>
     <row r="12" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B12">
         <v>1</v>
@@ -3612,7 +3612,7 @@
     </row>
     <row r="13" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B13">
         <v>1</v>

</xml_diff>

<commit_message>
v0.4.0 - Student life enhance
</commit_message>
<xml_diff>
--- a/Inputs/University.xlsx
+++ b/Inputs/University.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hbonn\Desktop\ESILV\A4\PI2\GitHub_PI2\Inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A67B9C4E-82F7-4509-9627-FD914A35447C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DBC0C69-A68A-4C2D-A9C9-B74D800B7E2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-34170" yWindow="-2700" windowWidth="24255" windowHeight="16575" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="University" sheetId="1" r:id="rId1"/>
@@ -939,7 +939,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
@@ -1127,8 +1127,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1143,7 +1143,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="B2" t="s">
         <v>14</v>
@@ -1151,7 +1151,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B3" t="s">
         <v>14</v>
@@ -1159,7 +1159,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B4" t="s">
         <v>14</v>
@@ -1167,7 +1167,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>176</v>
+        <v>16</v>
       </c>
       <c r="B5" t="s">
         <v>14</v>
@@ -1175,7 +1175,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B6" t="s">
         <v>14</v>
@@ -1183,7 +1183,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B7" t="s">
         <v>14</v>
@@ -1191,7 +1191,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>17</v>
+        <v>178</v>
       </c>
       <c r="B8" t="s">
         <v>14</v>

</xml_diff>

<commit_message>
Updates in the submodule
</commit_message>
<xml_diff>
--- a/Inputs/University.xlsx
+++ b/Inputs/University.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hbonn\Desktop\ESILV\A4\PI2\GitHub_PI2\Inputs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zinii\PI2_Project\Goodwing-Timetabler-Frontend-Plugins\Goodwing-Timetabler\Inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DBC0C69-A68A-4C2D-A9C9-B74D800B7E2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{878C15AD-217B-42CC-8A76-6128913565D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="University" sheetId="1" r:id="rId1"/>
@@ -182,12 +182,6 @@
     <t>Subjects (séparés d'un '-')</t>
   </si>
   <si>
-    <t>Henri</t>
-  </si>
-  <si>
-    <t>Barbeau</t>
-  </si>
-  <si>
     <t>Timothé</t>
   </si>
   <si>
@@ -579,6 +573,12 @@
   </si>
   <si>
     <t>TDC</t>
+  </si>
+  <si>
+    <t>Ilan</t>
+  </si>
+  <si>
+    <t>Zini</t>
   </si>
 </sst>
 </file>
@@ -943,7 +943,7 @@
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -1004,7 +1004,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -1127,11 +1127,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -1175,7 +1175,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B6" t="s">
         <v>14</v>
@@ -1183,7 +1183,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="B7" t="s">
         <v>14</v>
@@ -1191,7 +1191,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="B8" t="s">
         <v>14</v>
@@ -1210,7 +1210,7 @@
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -1220,7 +1220,7 @@
         <v>19</v>
       </c>
       <c r="C1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
@@ -1228,10 +1228,10 @@
         <v>20</v>
       </c>
       <c r="B2" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C2" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
   </sheetData>
@@ -1247,7 +1247,7 @@
       <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="36.33203125" customWidth="1"/>
     <col min="3" max="3" width="11.88671875" customWidth="1"/>
@@ -1325,10 +1325,10 @@
     </row>
     <row r="5" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>18</v>
@@ -1337,15 +1337,15 @@
         <v>15</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>18</v>
@@ -1354,15 +1354,15 @@
         <v>9</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>18</v>
@@ -1371,7 +1371,7 @@
         <v>15</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -1427,10 +1427,10 @@
     </row>
     <row r="11" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>19</v>
@@ -1439,15 +1439,15 @@
         <v>12</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>19</v>
@@ -1456,15 +1456,15 @@
         <v>12</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>19</v>
@@ -1473,103 +1473,103 @@
         <v>15</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D14" s="2">
         <v>24</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D15" s="2">
         <v>27</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D16" s="2">
         <v>27</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D17" s="2">
         <v>30</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D18" s="2">
         <v>21</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D19" s="2">
         <v>30</v>
@@ -1587,11 +1587,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="13.77734375" customWidth="1"/>
     <col min="3" max="3" width="16.44140625" customWidth="1"/>
@@ -1617,13 +1617,13 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>47</v>
+        <v>178</v>
       </c>
       <c r="C2" t="s">
-        <v>48</v>
+        <v>179</v>
       </c>
       <c r="D2" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -1631,13 +1631,13 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D3" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -1645,13 +1645,13 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="13.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -1659,13 +1659,13 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C5" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -1673,13 +1673,13 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="C6" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -1687,13 +1687,13 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C7" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
@@ -1701,13 +1701,13 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C8" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D8" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
@@ -1715,13 +1715,13 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C9" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D9" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
@@ -1729,13 +1729,13 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
+        <v>157</v>
+      </c>
+      <c r="C10" t="s">
+        <v>158</v>
+      </c>
+      <c r="D10" t="s">
         <v>159</v>
-      </c>
-      <c r="C10" t="s">
-        <v>160</v>
-      </c>
-      <c r="D10" t="s">
-        <v>161</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
@@ -1743,13 +1743,13 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="C11" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="D11" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
@@ -1757,13 +1757,13 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
+        <v>162</v>
+      </c>
+      <c r="C12" t="s">
+        <v>163</v>
+      </c>
+      <c r="D12" t="s">
         <v>164</v>
-      </c>
-      <c r="C12" t="s">
-        <v>165</v>
-      </c>
-      <c r="D12" t="s">
-        <v>166</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -1771,13 +1771,13 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="C13" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="D13" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
   </sheetData>
@@ -1793,7 +1793,7 @@
       <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="15" customWidth="1"/>
     <col min="2" max="49" width="12" customWidth="1"/>
@@ -1801,159 +1801,159 @@
   <sheetData>
     <row r="1" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C1" t="s">
         <v>59</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
         <v>60</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>61</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>62</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>63</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>64</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>65</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
         <v>66</v>
       </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
         <v>67</v>
       </c>
-      <c r="J1" t="s">
+      <c r="L1" t="s">
         <v>68</v>
       </c>
-      <c r="K1" t="s">
+      <c r="M1" t="s">
         <v>69</v>
       </c>
-      <c r="L1" t="s">
+      <c r="N1" t="s">
         <v>70</v>
       </c>
-      <c r="M1" t="s">
+      <c r="O1" t="s">
         <v>71</v>
       </c>
-      <c r="N1" t="s">
+      <c r="P1" t="s">
         <v>72</v>
       </c>
-      <c r="O1" t="s">
+      <c r="Q1" t="s">
         <v>73</v>
       </c>
-      <c r="P1" t="s">
+      <c r="R1" t="s">
         <v>74</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="S1" t="s">
         <v>75</v>
       </c>
-      <c r="R1" t="s">
+      <c r="T1" t="s">
         <v>76</v>
       </c>
-      <c r="S1" t="s">
+      <c r="U1" t="s">
         <v>77</v>
       </c>
-      <c r="T1" t="s">
+      <c r="V1" t="s">
         <v>78</v>
       </c>
-      <c r="U1" t="s">
+      <c r="W1" t="s">
         <v>79</v>
       </c>
-      <c r="V1" t="s">
+      <c r="X1" t="s">
         <v>80</v>
       </c>
-      <c r="W1" t="s">
+      <c r="Y1" t="s">
         <v>81</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Z1" t="s">
         <v>82</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="AA1" t="s">
         <v>83</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AB1" t="s">
         <v>84</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AC1" t="s">
         <v>85</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AD1" t="s">
         <v>86</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AE1" t="s">
         <v>87</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AF1" t="s">
         <v>88</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="AG1" t="s">
         <v>89</v>
       </c>
-      <c r="AF1" t="s">
+      <c r="AH1" t="s">
         <v>90</v>
       </c>
-      <c r="AG1" t="s">
+      <c r="AI1" t="s">
         <v>91</v>
       </c>
-      <c r="AH1" t="s">
+      <c r="AJ1" t="s">
         <v>92</v>
       </c>
-      <c r="AI1" t="s">
+      <c r="AK1" t="s">
         <v>93</v>
       </c>
-      <c r="AJ1" t="s">
+      <c r="AL1" t="s">
         <v>94</v>
       </c>
-      <c r="AK1" t="s">
+      <c r="AM1" t="s">
         <v>95</v>
       </c>
-      <c r="AL1" t="s">
+      <c r="AN1" t="s">
         <v>96</v>
       </c>
-      <c r="AM1" t="s">
+      <c r="AO1" t="s">
         <v>97</v>
       </c>
-      <c r="AN1" t="s">
+      <c r="AP1" t="s">
         <v>98</v>
       </c>
-      <c r="AO1" t="s">
+      <c r="AQ1" t="s">
         <v>99</v>
       </c>
-      <c r="AP1" t="s">
+      <c r="AR1" t="s">
         <v>100</v>
       </c>
-      <c r="AQ1" t="s">
+      <c r="AS1" t="s">
         <v>101</v>
       </c>
-      <c r="AR1" t="s">
+      <c r="AT1" t="s">
         <v>102</v>
       </c>
-      <c r="AS1" t="s">
+      <c r="AU1" t="s">
         <v>103</v>
       </c>
-      <c r="AT1" t="s">
+      <c r="AV1" t="s">
         <v>104</v>
       </c>
-      <c r="AU1" t="s">
+      <c r="AW1" t="s">
         <v>105</v>
       </c>
-      <c r="AV1" t="s">
+      <c r="AX1" t="s">
         <v>106</v>
-      </c>
-      <c r="AW1" t="s">
-        <v>107</v>
-      </c>
-      <c r="AX1" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="2" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -2105,7 +2105,7 @@
     </row>
     <row r="3" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -2257,7 +2257,7 @@
     </row>
     <row r="4" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -2409,7 +2409,7 @@
     </row>
     <row r="5" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -2561,7 +2561,7 @@
     </row>
     <row r="6" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -2713,7 +2713,7 @@
     </row>
     <row r="7" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -2865,7 +2865,7 @@
     </row>
     <row r="8" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B8">
         <v>1</v>
@@ -3017,7 +3017,7 @@
     </row>
     <row r="9" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -3169,7 +3169,7 @@
     </row>
     <row r="10" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B10">
         <v>1</v>
@@ -3321,7 +3321,7 @@
     </row>
     <row r="11" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B11">
         <v>1</v>
@@ -3473,7 +3473,7 @@
     </row>
     <row r="12" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B12">
         <v>1</v>
@@ -3625,7 +3625,7 @@
     </row>
     <row r="13" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B13">
         <v>1</v>
@@ -3777,7 +3777,7 @@
     </row>
     <row r="15" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
   </sheetData>

</xml_diff>